<commit_message>
navbars, footer, imgs and SiteInfo
</commit_message>
<xml_diff>
--- a/document/Foreservation_ViewList.xlsx
+++ b/document/Foreservation_ViewList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github_Intern2019\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA240E0-BC87-4F16-96E9-627E98149B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A18D5EB-AC16-4F02-A40B-7D8BAA78379C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-252" yWindow="2016" windowWidth="13488" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="View" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="289">
   <si>
     <t>OBJECT</t>
   </si>
@@ -672,10 +672,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Futter</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Acnt_RegAgr</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -815,18 +811,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ResrvNav</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SiteNav</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MyNav</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Mypage</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -999,19 +983,43 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>RoomNav</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>프로그램안내</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ProgramNav</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ProgramInfo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Footer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NavResrv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NavSite</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NavMain</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NavRoom</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NavProgram</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NavMy</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1060,7 +1068,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1070,6 +1078,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1138,7 +1152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1167,6 +1181,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1176,10 +1196,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1521,10 +1547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DF753CA-3B43-42CB-99AB-2EC6963C2F06}">
-  <dimension ref="A1:H84"/>
+  <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F61" sqref="F61"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.2" x14ac:dyDescent="0.45"/>
@@ -1540,22 +1566,22 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>167</v>
@@ -1565,1433 +1591,1288 @@
       </c>
     </row>
     <row r="2" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="5">
-        <v>1</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>275</v>
-      </c>
-      <c r="C2" s="14" t="s">
+      <c r="A2" s="5"/>
+      <c r="B2" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>176</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="E2" s="5" t="str">
+        <v>285</v>
+      </c>
+      <c r="E2" s="18" t="str">
         <f>D2&amp;".jsp"</f>
-        <v>ResrvNav.jsp</v>
+        <v>NavMain.jsp</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>235</v>
+        <v>284</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="14"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="11"/>
       <c r="D3" s="5" t="s">
-        <v>238</v>
+        <v>282</v>
       </c>
       <c r="E3" s="5" t="str">
-        <f t="shared" ref="E3" si="0">D3&amp;".jsp"</f>
-        <v>SiteNav.jsp</v>
+        <f>D3&amp;".jsp"</f>
+        <v>NavResrv.jsp</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>282</v>
+        <v>234</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
     </row>
     <row r="4" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="5">
-        <v>2</v>
-      </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="14"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="11"/>
       <c r="D4" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="E4" s="5" t="str">
-        <f>D4&amp;".jsp"</f>
-        <v>RoomNav.jsp</v>
+      <c r="E4" s="18" t="str">
+        <f t="shared" ref="E4" si="0">D4&amp;".jsp"</f>
+        <v>NavSite.jsp</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>236</v>
+        <v>278</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" s="5"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="14"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="11"/>
       <c r="D5" s="5" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="E5" s="5" t="str">
         <f>D5&amp;".jsp"</f>
-        <v>ProgramNav.jsp</v>
+        <v>NavRoom.jsp</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>284</v>
+        <v>235</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="5">
-        <v>3</v>
-      </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="14"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="11"/>
       <c r="D6" s="5" t="s">
-        <v>239</v>
+        <v>287</v>
       </c>
       <c r="E6" s="5" t="str">
-        <f t="shared" ref="E6:E68" si="1">D6&amp;".jsp"</f>
-        <v>MyNav.jsp</v>
+        <f>D6&amp;".jsp"</f>
+        <v>NavProgram.jsp</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>229</v>
+        <v>279</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="5">
-        <v>4</v>
-      </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="5" t="s">
-        <v>174</v>
-      </c>
+      <c r="A7" s="5"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="11"/>
       <c r="D7" s="5" t="s">
-        <v>201</v>
+        <v>288</v>
       </c>
       <c r="E7" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>Futter.jsp</v>
-      </c>
-      <c r="F7" s="9"/>
+        <f t="shared" ref="E7:E69" si="1">D7&amp;".jsp"</f>
+        <v>NavMy.jsp</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>228</v>
+      </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="5">
-        <v>5</v>
-      </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="14" t="s">
+      <c r="A8" s="5"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="E8" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>Footer.jsp</v>
+      </c>
+      <c r="F8" s="9"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="5"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D9" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="E8" s="10" t="str">
+      <c r="E9" s="15" t="str">
         <f t="shared" si="1"/>
         <v>ForeservationInfo.jsp</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F9" s="9" t="s">
         <v>177</v>
-      </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="5">
-        <v>6</v>
-      </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="9" t="s">
-        <v>179</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="5">
-        <v>7</v>
-      </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="12"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="16"/>
       <c r="F10" s="9" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="5">
-        <v>8</v>
-      </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="5" t="s">
+      <c r="A11" s="5"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="5"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D12" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="E11" s="5" t="str">
+      <c r="E12" s="5" t="str">
         <f t="shared" si="1"/>
         <v>SiteInfo.jsp</v>
-      </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="5">
-        <v>9</v>
-      </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="E12" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>RoomInfo.jsp</v>
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="5">
-        <v>10</v>
-      </c>
-      <c r="B13" s="11"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="13"/>
       <c r="C13" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>286</v>
+        <v>181</v>
       </c>
       <c r="E13" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>ProgramInfo.jsp</v>
+        <v>RoomInfo.jsp</v>
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="5">
-        <v>11</v>
-      </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="14" t="s">
+      <c r="A14" s="5"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="E14" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>ProgramInfo.jsp</v>
+      </c>
+      <c r="F14" s="9"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="5"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D15" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="E14" s="10" t="str">
+      <c r="E15" s="12" t="str">
         <f t="shared" si="1"/>
         <v>Login.jsp</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F15" s="9" t="s">
         <v>172</v>
-      </c>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-    </row>
-    <row r="15" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="5">
-        <v>12</v>
-      </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="9" t="s">
-        <v>197</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="5">
-        <v>13</v>
-      </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="11"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="13"/>
       <c r="F16" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="5">
-        <v>14</v>
-      </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="11"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="13"/>
       <c r="F17" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
     </row>
     <row r="18" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="5">
-        <v>15</v>
-      </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="12"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="13"/>
       <c r="F18" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="5">
-        <v>16</v>
-      </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="14" t="s">
+      <c r="A19" s="5"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="5"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="E19" s="5" t="str">
+      <c r="D20" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="E20" s="5" t="str">
         <f t="shared" si="1"/>
         <v>Acnt_RegAgr.jsp</v>
       </c>
-      <c r="F19" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-    </row>
-    <row r="20" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="5">
-        <v>17</v>
-      </c>
-      <c r="B20" s="11"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="E20" s="5" t="str">
+      <c r="F20" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="5"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="E21" s="5" t="str">
         <f t="shared" si="1"/>
         <v>Acnt_RegChk.jsp</v>
       </c>
-      <c r="F20" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-    </row>
-    <row r="21" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="5">
-        <v>18</v>
-      </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="E21" s="5" t="str">
+      <c r="F21" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="5"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="E22" s="5" t="str">
         <f t="shared" si="1"/>
         <v>Acnt_RegInfo.jsp</v>
       </c>
-      <c r="F21" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-    </row>
-    <row r="22" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="5">
-        <v>19</v>
-      </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="E22" s="5" t="str">
+      <c r="F22" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="5"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="E23" s="5" t="str">
         <f t="shared" si="1"/>
         <v>Acnt_RegCom.jsp</v>
       </c>
-      <c r="F22" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A23" s="5">
-        <v>20</v>
-      </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="13" t="s">
+      <c r="F23" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A24" s="5"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D24" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="E23" s="10" t="str">
+      <c r="E24" s="12" t="str">
         <f t="shared" si="1"/>
         <v>Foreservation.jsp</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F24" s="3" t="s">
         <v>169</v>
-      </c>
-      <c r="G23" s="3"/>
-      <c r="H23" s="1"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A24" s="5">
-        <v>21</v>
-      </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="3" t="s">
-        <v>168</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A25" s="5">
-        <v>22</v>
-      </c>
-      <c r="B25" s="11"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="11"/>
+      <c r="A25" s="5"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="13"/>
       <c r="F25" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A26" s="5">
-        <v>23</v>
-      </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="11"/>
+      <c r="A26" s="5"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="13"/>
       <c r="F26" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G26" s="3"/>
       <c r="H26" s="1"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A27" s="5">
-        <v>24</v>
-      </c>
-      <c r="B27" s="11"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="12"/>
+      <c r="A27" s="5"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="13"/>
       <c r="F27" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="1"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A28" s="5">
-        <v>25</v>
-      </c>
-      <c r="B28" s="11"/>
-      <c r="C28" s="13" t="s">
-        <v>210</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="E28" s="10" t="str">
+      <c r="A28" s="5"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="G28" s="3"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A29" s="5"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="E29" s="12" t="str">
         <f t="shared" si="1"/>
         <v>GnrSrch.jsp</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F29" s="3" t="s">
         <v>186</v>
-      </c>
-      <c r="G28" s="3"/>
-      <c r="H28" s="1"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A29" s="5">
-        <v>26</v>
-      </c>
-      <c r="B29" s="11"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="3" t="s">
-        <v>187</v>
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="1"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A30" s="5">
-        <v>27</v>
-      </c>
-      <c r="B30" s="11"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="11"/>
+      <c r="A30" s="5"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="13"/>
       <c r="F30" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G30" s="3"/>
       <c r="H30" s="1"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A31" s="5">
-        <v>28</v>
-      </c>
-      <c r="B31" s="11"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="11"/>
+      <c r="A31" s="5"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="13"/>
       <c r="F31" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="1"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A32" s="5">
-        <v>29</v>
-      </c>
-      <c r="B32" s="11"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="8" t="s">
-        <v>194</v>
+      <c r="A32" s="5"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="3" t="s">
+        <v>190</v>
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="1"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A33" s="5">
-        <v>30</v>
-      </c>
-      <c r="B33" s="11"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="3" t="s">
-        <v>188</v>
+      <c r="A33" s="5"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="8" t="s">
+        <v>194</v>
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="1"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A34" s="5">
-        <v>31</v>
-      </c>
-      <c r="B34" s="11"/>
-      <c r="C34" s="13" t="s">
+      <c r="A34" s="5"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="G34" s="3"/>
+      <c r="H34" s="1"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A35" s="5"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="D34" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="E34" s="10" t="str">
+      <c r="D35" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="E35" s="12" t="str">
         <f t="shared" si="1"/>
         <v>MonthSrch.jsp</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F35" s="3" t="s">
         <v>186</v>
-      </c>
-      <c r="G34" s="3"/>
-      <c r="H34" s="1"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A35" s="5">
-        <v>32</v>
-      </c>
-      <c r="B35" s="11"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="3" t="s">
-        <v>187</v>
       </c>
       <c r="G35" s="3"/>
       <c r="H35" s="1"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A36" s="5">
-        <v>33</v>
-      </c>
-      <c r="B36" s="11"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="12"/>
+      <c r="A36" s="5"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="13"/>
       <c r="F36" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="G36" s="3"/>
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A37" s="5"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="G36" s="3"/>
-      <c r="H36" s="1" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A37" s="5">
-        <v>34</v>
-      </c>
-      <c r="B37" s="11"/>
-      <c r="C37" s="13" t="s">
+      <c r="G37" s="3"/>
+      <c r="H37" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A38" s="5"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="D37" s="13" t="s">
+      <c r="D38" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="E37" s="10" t="str">
+      <c r="E38" s="12" t="str">
         <f t="shared" si="1"/>
         <v>GnrResrv.jsp</v>
       </c>
-      <c r="F37" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="G37" s="3"/>
-      <c r="H37" s="1"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A38" s="5">
-        <v>35</v>
-      </c>
-      <c r="B38" s="11"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="11"/>
       <c r="F38" s="3" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="G38" s="3"/>
       <c r="H38" s="1"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A39" s="5">
-        <v>36</v>
-      </c>
-      <c r="B39" s="11"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="11"/>
+      <c r="A39" s="5"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="13"/>
       <c r="F39" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G39" s="3"/>
       <c r="H39" s="1"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A40" s="5">
-        <v>37</v>
-      </c>
-      <c r="B40" s="11"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="11"/>
+      <c r="A40" s="5"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="13"/>
       <c r="F40" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G40" s="3"/>
       <c r="H40" s="1"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A41" s="5">
-        <v>38</v>
-      </c>
-      <c r="B41" s="11"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="8" t="s">
-        <v>218</v>
+      <c r="A41" s="5"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="3" t="s">
+        <v>216</v>
       </c>
       <c r="G41" s="3"/>
       <c r="H41" s="1"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A42" s="5">
-        <v>39</v>
-      </c>
-      <c r="B42" s="11"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="3" t="s">
+      <c r="A42" s="5"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="G42" s="3"/>
+      <c r="H42" s="1"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A43" s="5"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="G42" s="3"/>
-      <c r="H42" s="1" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A43" s="5">
-        <v>40</v>
-      </c>
-      <c r="B43" s="11"/>
-      <c r="C43" s="13" t="s">
-        <v>211</v>
-      </c>
-      <c r="D43" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="E43" s="10" t="str">
+      <c r="G43" s="3"/>
+      <c r="H43" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A44" s="5"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="E44" s="12" t="str">
         <f t="shared" si="1"/>
         <v>PrgmSrch.jsp</v>
       </c>
-      <c r="F43" s="3" t="s">
+      <c r="F44" s="3" t="s">
         <v>186</v>
-      </c>
-      <c r="G43" s="3"/>
-      <c r="H43" s="1"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A44" s="5">
-        <v>41</v>
-      </c>
-      <c r="B44" s="11"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="11"/>
-      <c r="F44" s="3" t="s">
-        <v>187</v>
       </c>
       <c r="G44" s="3"/>
       <c r="H44" s="1"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A45" s="5">
-        <v>42</v>
-      </c>
-      <c r="B45" s="11"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="11"/>
+      <c r="A45" s="5"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="13"/>
       <c r="F45" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G45" s="3"/>
       <c r="H45" s="1"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A46" s="5">
-        <v>43</v>
-      </c>
-      <c r="B46" s="11"/>
-      <c r="C46" s="13"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="11"/>
+      <c r="A46" s="5"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="13"/>
       <c r="F46" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G46" s="3"/>
       <c r="H46" s="1"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A47" s="5">
-        <v>44</v>
-      </c>
-      <c r="B47" s="11"/>
-      <c r="C47" s="13"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="8" t="s">
-        <v>193</v>
+      <c r="A47" s="5"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="3" t="s">
+        <v>190</v>
       </c>
       <c r="G47" s="3"/>
       <c r="H47" s="1"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A48" s="5">
-        <v>45</v>
-      </c>
-      <c r="B48" s="11"/>
-      <c r="C48" s="13" t="s">
+      <c r="A48" s="5"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="G48" s="3"/>
+      <c r="H48" s="1"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A49" s="5"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="D48" s="13" t="s">
+      <c r="D49" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="E48" s="10" t="str">
+      <c r="E49" s="12" t="str">
         <f t="shared" si="1"/>
         <v>PrgmResrv.jsp</v>
       </c>
-      <c r="F48" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="G48" s="3"/>
-      <c r="H48" s="1"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A49" s="5">
-        <v>46</v>
-      </c>
-      <c r="B49" s="11"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="11"/>
       <c r="F49" s="3" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="G49" s="3"/>
       <c r="H49" s="1"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A50" s="5">
-        <v>47</v>
-      </c>
-      <c r="B50" s="11"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="11"/>
+      <c r="A50" s="5"/>
+      <c r="B50" s="13"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="13"/>
       <c r="F50" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G50" s="3"/>
       <c r="H50" s="1"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A51" s="5">
-        <v>48</v>
-      </c>
-      <c r="B51" s="11"/>
-      <c r="C51" s="13"/>
-      <c r="D51" s="13"/>
-      <c r="E51" s="11"/>
+      <c r="A51" s="5"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="13"/>
       <c r="F51" s="3" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G51" s="3"/>
       <c r="H51" s="1"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A52" s="5">
-        <v>49</v>
-      </c>
-      <c r="B52" s="11"/>
-      <c r="C52" s="13"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="12"/>
+      <c r="A52" s="5"/>
+      <c r="B52" s="13"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="13"/>
       <c r="F52" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="G52" s="3"/>
+      <c r="H52" s="1"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A53" s="5"/>
+      <c r="B53" s="13"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="G52" s="3"/>
-      <c r="H52" s="1" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A53" s="5">
-        <v>50</v>
-      </c>
-      <c r="B53" s="11"/>
-      <c r="C53" s="13" t="s">
+      <c r="G53" s="3"/>
+      <c r="H53" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A54" s="5"/>
+      <c r="B54" s="13"/>
+      <c r="C54" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="D54" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="D53" s="13" t="s">
-        <v>224</v>
-      </c>
-      <c r="E53" s="10" t="str">
+      <c r="E54" s="12" t="str">
         <f t="shared" si="1"/>
         <v>PayInfo.jsp</v>
       </c>
-      <c r="F53" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="G53" s="3"/>
-      <c r="H53" s="1"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A54" s="5">
-        <v>51</v>
-      </c>
-      <c r="B54" s="11"/>
-      <c r="C54" s="13"/>
-      <c r="D54" s="13"/>
-      <c r="E54" s="11"/>
       <c r="F54" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G54" s="3"/>
       <c r="H54" s="1"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A55" s="5">
-        <v>52</v>
-      </c>
-      <c r="B55" s="11"/>
-      <c r="C55" s="13"/>
-      <c r="D55" s="13"/>
-      <c r="E55" s="11"/>
+      <c r="A55" s="5"/>
+      <c r="B55" s="13"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="13"/>
       <c r="F55" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G55" s="3"/>
       <c r="H55" s="1"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A56" s="5">
-        <v>53</v>
-      </c>
-      <c r="B56" s="11"/>
-      <c r="C56" s="13"/>
-      <c r="D56" s="13"/>
-      <c r="E56" s="11"/>
+      <c r="A56" s="5"/>
+      <c r="B56" s="13"/>
+      <c r="C56" s="10"/>
+      <c r="D56" s="10"/>
+      <c r="E56" s="13"/>
       <c r="F56" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G56" s="3"/>
       <c r="H56" s="1"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A57" s="5">
-        <v>54</v>
-      </c>
-      <c r="B57" s="11"/>
-      <c r="C57" s="13"/>
-      <c r="D57" s="13"/>
-      <c r="E57" s="12"/>
+      <c r="A57" s="5"/>
+      <c r="B57" s="13"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="13"/>
       <c r="F57" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G57" s="3"/>
       <c r="H57" s="1"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A58" s="5">
-        <v>55</v>
-      </c>
-      <c r="B58" s="11"/>
-      <c r="C58" s="1" t="s">
+      <c r="A58" s="5"/>
+      <c r="B58" s="13"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="10"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="G58" s="3"/>
+      <c r="H58" s="1"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A59" s="5"/>
+      <c r="B59" s="13"/>
+      <c r="C59" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="D58" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="E58" s="5" t="str">
+      <c r="E59" s="5" t="str">
         <f t="shared" si="1"/>
         <v>PayCmplt.jsp</v>
       </c>
-      <c r="F58" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="G58" s="3"/>
-      <c r="H58" s="1"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A59" s="5">
-        <v>56</v>
-      </c>
-      <c r="B59" s="11"/>
-      <c r="C59" s="13" t="s">
-        <v>229</v>
-      </c>
-      <c r="D59" s="13" t="s">
-        <v>240</v>
-      </c>
-      <c r="E59" s="10" t="str">
+      <c r="F59" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="G59" s="3"/>
+      <c r="H59" s="1"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A60" s="5"/>
+      <c r="B60" s="13"/>
+      <c r="C60" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="E60" s="12" t="str">
         <f t="shared" si="1"/>
         <v>Mypage.jsp</v>
       </c>
-      <c r="F59" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="G59" s="3"/>
-      <c r="H59" s="1"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A60" s="5">
-        <v>57</v>
-      </c>
-      <c r="B60" s="11"/>
-      <c r="C60" s="13"/>
-      <c r="D60" s="13"/>
-      <c r="E60" s="11"/>
       <c r="F60" s="3" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="G60" s="3"/>
       <c r="H60" s="1"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A61" s="5">
-        <v>58</v>
-      </c>
-      <c r="B61" s="11"/>
-      <c r="C61" s="13"/>
-      <c r="D61" s="13"/>
-      <c r="E61" s="11"/>
+      <c r="A61" s="5"/>
+      <c r="B61" s="13"/>
+      <c r="C61" s="10"/>
+      <c r="D61" s="10"/>
+      <c r="E61" s="13"/>
       <c r="F61" s="3" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="G61" s="3"/>
       <c r="H61" s="1"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A62" s="5">
-        <v>59</v>
-      </c>
-      <c r="B62" s="11"/>
-      <c r="C62" s="13"/>
-      <c r="D62" s="13"/>
-      <c r="E62" s="11"/>
+      <c r="A62" s="5"/>
+      <c r="B62" s="13"/>
+      <c r="C62" s="10"/>
+      <c r="D62" s="10"/>
+      <c r="E62" s="13"/>
       <c r="F62" s="3" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="G62" s="3"/>
       <c r="H62" s="1"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A63" s="5">
-        <v>60</v>
-      </c>
-      <c r="B63" s="11"/>
-      <c r="C63" s="13"/>
-      <c r="D63" s="13"/>
-      <c r="E63" s="12"/>
+      <c r="A63" s="5"/>
+      <c r="B63" s="13"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="10"/>
+      <c r="E63" s="13"/>
       <c r="F63" s="3" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="G63" s="3"/>
       <c r="H63" s="1"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A64" s="5">
-        <v>61</v>
-      </c>
-      <c r="B64" s="11"/>
-      <c r="C64" s="13" t="s">
+      <c r="A64" s="5"/>
+      <c r="B64" s="13"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="10"/>
+      <c r="E64" s="14"/>
+      <c r="F64" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="D64" s="13" t="s">
-        <v>246</v>
-      </c>
-      <c r="E64" s="10" t="str">
+      <c r="G64" s="3"/>
+      <c r="H64" s="1"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A65" s="5"/>
+      <c r="B65" s="13"/>
+      <c r="C65" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="D65" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="E65" s="12" t="str">
         <f t="shared" si="1"/>
         <v>MyResrv.jsp</v>
       </c>
-      <c r="F64" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="G64" s="3"/>
-      <c r="H64" s="1"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A65" s="5">
-        <v>62</v>
-      </c>
-      <c r="B65" s="11"/>
-      <c r="C65" s="13"/>
-      <c r="D65" s="13"/>
-      <c r="E65" s="11"/>
       <c r="F65" s="3" t="s">
-        <v>228</v>
+        <v>243</v>
       </c>
       <c r="G65" s="3"/>
       <c r="H65" s="1"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A66" s="5">
-        <v>63</v>
-      </c>
-      <c r="B66" s="11"/>
-      <c r="C66" s="13"/>
-      <c r="D66" s="13"/>
-      <c r="E66" s="11"/>
+      <c r="A66" s="5"/>
+      <c r="B66" s="13"/>
+      <c r="C66" s="10"/>
+      <c r="D66" s="10"/>
+      <c r="E66" s="13"/>
       <c r="F66" s="3" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="G66" s="3"/>
       <c r="H66" s="1"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A67" s="5">
-        <v>64</v>
-      </c>
-      <c r="B67" s="11"/>
-      <c r="C67" s="13"/>
-      <c r="D67" s="13"/>
-      <c r="E67" s="12"/>
+      <c r="A67" s="5"/>
+      <c r="B67" s="13"/>
+      <c r="C67" s="10"/>
+      <c r="D67" s="10"/>
+      <c r="E67" s="13"/>
       <c r="F67" s="3" t="s">
-        <v>248</v>
+        <v>229</v>
       </c>
       <c r="G67" s="3"/>
       <c r="H67" s="1"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A68" s="5">
-        <v>65</v>
-      </c>
-      <c r="B68" s="11"/>
-      <c r="C68" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="D68" s="13" t="s">
-        <v>250</v>
-      </c>
-      <c r="E68" s="10" t="str">
+      <c r="A68" s="5"/>
+      <c r="B68" s="13"/>
+      <c r="C68" s="10"/>
+      <c r="D68" s="10"/>
+      <c r="E68" s="14"/>
+      <c r="F68" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="G68" s="3"/>
+      <c r="H68" s="1"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A69" s="5"/>
+      <c r="B69" s="13"/>
+      <c r="C69" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="D69" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="E69" s="12" t="str">
         <f t="shared" si="1"/>
         <v>ResrvCancle.jsp</v>
       </c>
-      <c r="F68" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="G68" s="3"/>
-      <c r="H68" s="1"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A69" s="5">
-        <v>66</v>
-      </c>
-      <c r="B69" s="11"/>
-      <c r="C69" s="13"/>
-      <c r="D69" s="13"/>
-      <c r="E69" s="12"/>
       <c r="F69" s="3" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="G69" s="3"/>
       <c r="H69" s="1"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A70" s="5">
-        <v>67</v>
-      </c>
-      <c r="B70" s="11"/>
-      <c r="C70" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="D70" s="13" t="s">
-        <v>258</v>
-      </c>
-      <c r="E70" s="10" t="str">
-        <f t="shared" ref="E70:E84" si="2">D70&amp;".jsp"</f>
-        <v>ResrvInfo.jsp</v>
-      </c>
+      <c r="A70" s="5"/>
+      <c r="B70" s="13"/>
+      <c r="C70" s="10"/>
+      <c r="D70" s="10"/>
+      <c r="E70" s="14"/>
       <c r="F70" s="3" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="G70" s="3"/>
       <c r="H70" s="1"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A71" s="5">
-        <v>68</v>
-      </c>
-      <c r="B71" s="11"/>
-      <c r="C71" s="13"/>
-      <c r="D71" s="13"/>
-      <c r="E71" s="11"/>
+      <c r="A71" s="5"/>
+      <c r="B71" s="13"/>
+      <c r="C71" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="D71" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="E71" s="12" t="str">
+        <f t="shared" ref="E71:E85" si="2">D71&amp;".jsp"</f>
+        <v>ResrvInfo.jsp</v>
+      </c>
       <c r="F71" s="3" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="G71" s="3"/>
       <c r="H71" s="1"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A72" s="5">
-        <v>69</v>
-      </c>
-      <c r="B72" s="11"/>
-      <c r="C72" s="13"/>
-      <c r="D72" s="13"/>
-      <c r="E72" s="11"/>
+      <c r="A72" s="5"/>
+      <c r="B72" s="13"/>
+      <c r="C72" s="10"/>
+      <c r="D72" s="10"/>
+      <c r="E72" s="13"/>
       <c r="F72" s="3" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G72" s="3"/>
       <c r="H72" s="1"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A73" s="5">
-        <v>70</v>
-      </c>
-      <c r="B73" s="11"/>
-      <c r="C73" s="13"/>
-      <c r="D73" s="13"/>
-      <c r="E73" s="12"/>
+      <c r="A73" s="5"/>
+      <c r="B73" s="13"/>
+      <c r="C73" s="10"/>
+      <c r="D73" s="10"/>
+      <c r="E73" s="13"/>
       <c r="F73" s="3" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="G73" s="3"/>
       <c r="H73" s="1"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A74" s="5">
-        <v>71</v>
-      </c>
-      <c r="B74" s="11"/>
-      <c r="C74" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="E74" s="5" t="str">
+      <c r="A74" s="5"/>
+      <c r="B74" s="13"/>
+      <c r="C74" s="10"/>
+      <c r="D74" s="10"/>
+      <c r="E74" s="14"/>
+      <c r="F74" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="G74" s="3"/>
+      <c r="H74" s="1"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A75" s="5"/>
+      <c r="B75" s="13"/>
+      <c r="C75" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="E75" s="5" t="str">
         <f t="shared" si="2"/>
         <v>JimList.jsp</v>
       </c>
-      <c r="F74" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="G74" s="3"/>
-      <c r="H74" s="1"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A75" s="5">
-        <v>72</v>
-      </c>
-      <c r="B75" s="11"/>
-      <c r="C75" s="13" t="s">
-        <v>261</v>
-      </c>
-      <c r="D75" s="13" t="s">
-        <v>262</v>
-      </c>
-      <c r="E75" s="10" t="str">
+      <c r="F75" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="G75" s="3"/>
+      <c r="H75" s="1"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A76" s="5"/>
+      <c r="B76" s="13"/>
+      <c r="C76" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="D76" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="E76" s="12" t="str">
         <f t="shared" si="2"/>
         <v>MyQnalist.jsp</v>
       </c>
-      <c r="F75" s="3" t="s">
+      <c r="F76" s="3" t="s">
         <v>186</v>
-      </c>
-      <c r="G75" s="3"/>
-      <c r="H75" s="1"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A76" s="5">
-        <v>73</v>
-      </c>
-      <c r="B76" s="11"/>
-      <c r="C76" s="13"/>
-      <c r="D76" s="13"/>
-      <c r="E76" s="11"/>
-      <c r="F76" s="3" t="s">
-        <v>263</v>
       </c>
       <c r="G76" s="3"/>
       <c r="H76" s="1"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A77" s="5">
-        <v>74</v>
-      </c>
-      <c r="B77" s="11"/>
-      <c r="C77" s="13"/>
-      <c r="D77" s="13"/>
-      <c r="E77" s="12"/>
+      <c r="A77" s="5"/>
+      <c r="B77" s="13"/>
+      <c r="C77" s="10"/>
+      <c r="D77" s="10"/>
+      <c r="E77" s="13"/>
       <c r="F77" s="3" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="G77" s="3"/>
       <c r="H77" s="1"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A78" s="5">
-        <v>75</v>
-      </c>
-      <c r="B78" s="11"/>
-      <c r="C78" s="13" t="s">
-        <v>265</v>
-      </c>
-      <c r="D78" s="13" t="s">
-        <v>266</v>
-      </c>
-      <c r="E78" s="10" t="str">
+      <c r="A78" s="5"/>
+      <c r="B78" s="13"/>
+      <c r="C78" s="10"/>
+      <c r="D78" s="10"/>
+      <c r="E78" s="14"/>
+      <c r="F78" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="G78" s="3"/>
+      <c r="H78" s="1"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A79" s="5"/>
+      <c r="B79" s="13"/>
+      <c r="C79" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="D79" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="E79" s="12" t="str">
         <f t="shared" si="2"/>
         <v>QnaReg.jsp</v>
       </c>
-      <c r="F78" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="G78" s="3"/>
-      <c r="H78" s="1"/>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A79" s="5">
-        <v>76</v>
-      </c>
-      <c r="B79" s="11"/>
-      <c r="C79" s="13"/>
-      <c r="D79" s="13"/>
-      <c r="E79" s="12"/>
       <c r="F79" s="3" t="s">
-        <v>252</v>
+        <v>263</v>
       </c>
       <c r="G79" s="3"/>
       <c r="H79" s="1"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A80" s="5">
-        <v>77</v>
-      </c>
-      <c r="B80" s="11"/>
-      <c r="C80" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="E80" s="5" t="str">
+      <c r="A80" s="5"/>
+      <c r="B80" s="13"/>
+      <c r="C80" s="10"/>
+      <c r="D80" s="10"/>
+      <c r="E80" s="14"/>
+      <c r="F80" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="G80" s="3"/>
+      <c r="H80" s="1"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A81" s="5"/>
+      <c r="B81" s="13"/>
+      <c r="C81" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E81" s="5" t="str">
         <f t="shared" si="2"/>
         <v>MyInfo.jsp</v>
       </c>
-      <c r="F80" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="G80" s="3"/>
-      <c r="H80" s="1"/>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A81" s="5">
-        <v>78</v>
-      </c>
-      <c r="B81" s="11"/>
-      <c r="C81" s="13" t="s">
-        <v>269</v>
-      </c>
-      <c r="D81" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="E81" s="10" t="str">
+      <c r="F81" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="G81" s="3"/>
+      <c r="H81" s="1"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A82" s="5"/>
+      <c r="B82" s="13"/>
+      <c r="C82" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="D82" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="E82" s="12" t="str">
         <f t="shared" si="2"/>
         <v>MyInfoEdit.jsp</v>
       </c>
-      <c r="F81" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="G81" s="3"/>
-      <c r="H81" s="1"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A82" s="5">
-        <v>79</v>
-      </c>
-      <c r="B82" s="11"/>
-      <c r="C82" s="13"/>
-      <c r="D82" s="13"/>
-      <c r="E82" s="11"/>
       <c r="F82" s="3" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="G82" s="3"/>
       <c r="H82" s="1"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A83" s="5">
-        <v>80</v>
-      </c>
-      <c r="B83" s="11"/>
-      <c r="C83" s="13"/>
-      <c r="D83" s="13"/>
-      <c r="E83" s="12"/>
+      <c r="A83" s="5"/>
+      <c r="B83" s="13"/>
+      <c r="C83" s="10"/>
+      <c r="D83" s="10"/>
+      <c r="E83" s="13"/>
       <c r="F83" s="3" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="G83" s="3"/>
       <c r="H83" s="1"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A84" s="5">
-        <v>81</v>
-      </c>
-      <c r="B84" s="12"/>
-      <c r="C84" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="E84" s="5" t="str">
+      <c r="A84" s="5"/>
+      <c r="B84" s="13"/>
+      <c r="C84" s="10"/>
+      <c r="D84" s="10"/>
+      <c r="E84" s="14"/>
+      <c r="F84" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="G84" s="3"/>
+      <c r="H84" s="1"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A85" s="5"/>
+      <c r="B85" s="14"/>
+      <c r="C85" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="E85" s="5" t="str">
         <f t="shared" si="2"/>
         <v>MyWidrw.jsp</v>
       </c>
-      <c r="F84" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="G84" s="3"/>
-      <c r="H84" s="1"/>
+      <c r="F85" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="G85" s="3"/>
+      <c r="H85" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="D37:D42"/>
-    <mergeCell ref="C37:C42"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="D68:D69"/>
-    <mergeCell ref="D43:D47"/>
-    <mergeCell ref="C53:C57"/>
-    <mergeCell ref="D53:D57"/>
-    <mergeCell ref="D48:D52"/>
-    <mergeCell ref="C48:C52"/>
-    <mergeCell ref="C43:C47"/>
-    <mergeCell ref="C2:C6"/>
-    <mergeCell ref="D59:D63"/>
-    <mergeCell ref="C59:C63"/>
-    <mergeCell ref="D64:D67"/>
-    <mergeCell ref="C64:C67"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="C14:C18"/>
-    <mergeCell ref="D14:D18"/>
-    <mergeCell ref="C19:C22"/>
-    <mergeCell ref="C28:C33"/>
-    <mergeCell ref="D28:D33"/>
-    <mergeCell ref="D23:D27"/>
-    <mergeCell ref="C23:C27"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D81:D83"/>
-    <mergeCell ref="C81:C83"/>
-    <mergeCell ref="B2:B84"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="E14:E18"/>
-    <mergeCell ref="E23:E27"/>
-    <mergeCell ref="E28:E33"/>
-    <mergeCell ref="E34:E36"/>
-    <mergeCell ref="E37:E42"/>
-    <mergeCell ref="E43:E47"/>
-    <mergeCell ref="C70:C73"/>
-    <mergeCell ref="D70:D73"/>
-    <mergeCell ref="D75:D77"/>
-    <mergeCell ref="C75:C77"/>
-    <mergeCell ref="D78:D79"/>
-    <mergeCell ref="C78:C79"/>
-    <mergeCell ref="E75:E77"/>
-    <mergeCell ref="E78:E79"/>
-    <mergeCell ref="E81:E83"/>
-    <mergeCell ref="E48:E52"/>
-    <mergeCell ref="E53:E57"/>
-    <mergeCell ref="E59:E63"/>
-    <mergeCell ref="E64:E67"/>
-    <mergeCell ref="E68:E69"/>
-    <mergeCell ref="E70:E73"/>
+    <mergeCell ref="E76:E78"/>
+    <mergeCell ref="E79:E80"/>
+    <mergeCell ref="E82:E84"/>
+    <mergeCell ref="E49:E53"/>
+    <mergeCell ref="E54:E58"/>
+    <mergeCell ref="E60:E64"/>
+    <mergeCell ref="E65:E68"/>
+    <mergeCell ref="E69:E70"/>
+    <mergeCell ref="E71:E74"/>
+    <mergeCell ref="D82:D84"/>
+    <mergeCell ref="C82:C84"/>
+    <mergeCell ref="B2:B85"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="E15:E19"/>
+    <mergeCell ref="E24:E28"/>
+    <mergeCell ref="E29:E34"/>
+    <mergeCell ref="E35:E37"/>
+    <mergeCell ref="E38:E43"/>
+    <mergeCell ref="E44:E48"/>
+    <mergeCell ref="C71:C74"/>
+    <mergeCell ref="D71:D74"/>
+    <mergeCell ref="D76:D78"/>
+    <mergeCell ref="C76:C78"/>
+    <mergeCell ref="D79:D80"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="C2:C7"/>
+    <mergeCell ref="D60:D64"/>
+    <mergeCell ref="C60:C64"/>
+    <mergeCell ref="D65:D68"/>
+    <mergeCell ref="C65:C68"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="D35:D37"/>
+    <mergeCell ref="C15:C19"/>
+    <mergeCell ref="D15:D19"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="C29:C34"/>
+    <mergeCell ref="D29:D34"/>
+    <mergeCell ref="D24:D28"/>
+    <mergeCell ref="C24:C28"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="D38:D43"/>
+    <mergeCell ref="C38:C43"/>
+    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="D69:D70"/>
+    <mergeCell ref="D44:D48"/>
+    <mergeCell ref="C54:C58"/>
+    <mergeCell ref="D54:D58"/>
+    <mergeCell ref="D49:D53"/>
+    <mergeCell ref="C49:C53"/>
+    <mergeCell ref="C44:C48"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
RoomInfo, ProgramInfo, Navbars and images
</commit_message>
<xml_diff>
--- a/document/Foreservation_ViewList.xlsx
+++ b/document/Foreservation_ViewList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github_Intern2019\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A18D5EB-AC16-4F02-A40B-7D8BAA78379C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5694EEC-D3EC-4B21-8481-30216C5ECD66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -999,10 +999,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>NavSite</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>메인</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1011,15 +1007,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>NavRoom</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NavProgram</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>NavMy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NavSiteInfo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NavRoomInfo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NavProgramInfo</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1181,10 +1181,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1196,6 +1193,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1205,7 +1205,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1550,7 +1550,7 @@
   <dimension ref="A1:H85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.2" x14ac:dyDescent="0.45"/>
@@ -1592,29 +1592,29 @@
     </row>
     <row r="2" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="5"/>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>271</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="18" t="s">
         <v>176</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="E2" s="18" t="str">
+        <v>284</v>
+      </c>
+      <c r="E2" s="10" t="str">
         <f>D2&amp;".jsp"</f>
         <v>NavMain.jsp</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="11"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="18"/>
       <c r="D3" s="5" t="s">
         <v>282</v>
       </c>
@@ -1630,14 +1630,14 @@
     </row>
     <row r="4" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="5"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="11"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="18"/>
       <c r="D4" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="E4" s="18" t="str">
-        <f t="shared" ref="E4" si="0">D4&amp;".jsp"</f>
-        <v>NavSite.jsp</v>
+        <v>286</v>
+      </c>
+      <c r="E4" s="10" t="str">
+        <f t="shared" ref="E4:E5" si="0">D4&amp;".jsp"</f>
+        <v>NavSiteInfo.jsp</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>278</v>
@@ -1647,14 +1647,14 @@
     </row>
     <row r="5" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" s="5"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="11"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="18"/>
       <c r="D5" s="5" t="s">
-        <v>286</v>
-      </c>
-      <c r="E5" s="5" t="str">
+        <v>287</v>
+      </c>
+      <c r="E5" s="10" t="str">
         <f>D5&amp;".jsp"</f>
-        <v>NavRoom.jsp</v>
+        <v>NavRoomInfo.jsp</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>235</v>
@@ -1664,14 +1664,14 @@
     </row>
     <row r="6" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A6" s="5"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="11"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="18"/>
       <c r="D6" s="5" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E6" s="5" t="str">
         <f>D6&amp;".jsp"</f>
-        <v>NavProgram.jsp</v>
+        <v>NavProgramInfo.jsp</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>279</v>
@@ -1681,10 +1681,10 @@
     </row>
     <row r="7" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A7" s="5"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="18"/>
       <c r="D7" s="5" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="E7" s="5" t="str">
         <f t="shared" ref="E7:E69" si="1">D7&amp;".jsp"</f>
@@ -1698,14 +1698,14 @@
     </row>
     <row r="8" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A8" s="5"/>
-      <c r="B8" s="13"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="5" t="s">
         <v>174</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="E8" s="18" t="str">
+      <c r="E8" s="10" t="str">
         <f t="shared" si="1"/>
         <v>Footer.jsp</v>
       </c>
@@ -1715,11 +1715,11 @@
     </row>
     <row r="9" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A9" s="5"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="11" t="s">
+      <c r="B9" s="12"/>
+      <c r="C9" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="18" t="s">
         <v>183</v>
       </c>
       <c r="E9" s="15" t="str">
@@ -1734,9 +1734,9 @@
     </row>
     <row r="10" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A10" s="5"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
       <c r="E10" s="16"/>
       <c r="F10" s="9" t="s">
         <v>179</v>
@@ -1746,9 +1746,9 @@
     </row>
     <row r="11" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A11" s="5"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
       <c r="E11" s="17"/>
       <c r="F11" s="9" t="s">
         <v>178</v>
@@ -1758,14 +1758,14 @@
     </row>
     <row r="12" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A12" s="5"/>
-      <c r="B12" s="13"/>
+      <c r="B12" s="12"/>
       <c r="C12" s="5" t="s">
         <v>177</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="E12" s="5" t="str">
+      <c r="E12" s="10" t="str">
         <f t="shared" si="1"/>
         <v>SiteInfo.jsp</v>
       </c>
@@ -1775,7 +1775,7 @@
     </row>
     <row r="13" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A13" s="5"/>
-      <c r="B13" s="13"/>
+      <c r="B13" s="12"/>
       <c r="C13" s="5" t="s">
         <v>179</v>
       </c>
@@ -1792,7 +1792,7 @@
     </row>
     <row r="14" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A14" s="5"/>
-      <c r="B14" s="13"/>
+      <c r="B14" s="12"/>
       <c r="C14" s="5" t="s">
         <v>178</v>
       </c>
@@ -1809,14 +1809,14 @@
     </row>
     <row r="15" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A15" s="5"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="11" t="s">
+      <c r="B15" s="12"/>
+      <c r="C15" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="18" t="s">
         <v>196</v>
       </c>
-      <c r="E15" s="12" t="str">
+      <c r="E15" s="11" t="str">
         <f t="shared" si="1"/>
         <v>Login.jsp</v>
       </c>
@@ -1828,10 +1828,10 @@
     </row>
     <row r="16" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A16" s="5"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="13"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="12"/>
       <c r="F16" s="9" t="s">
         <v>197</v>
       </c>
@@ -1840,10 +1840,10 @@
     </row>
     <row r="17" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A17" s="5"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="13"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="12"/>
       <c r="F17" s="9" t="s">
         <v>198</v>
       </c>
@@ -1852,10 +1852,10 @@
     </row>
     <row r="18" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A18" s="5"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="13"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="12"/>
       <c r="F18" s="9" t="s">
         <v>199</v>
       </c>
@@ -1864,10 +1864,10 @@
     </row>
     <row r="19" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A19" s="5"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="14"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="13"/>
       <c r="F19" s="9" t="s">
         <v>200</v>
       </c>
@@ -1876,8 +1876,8 @@
     </row>
     <row r="20" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A20" s="5"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="11" t="s">
+      <c r="B20" s="12"/>
+      <c r="C20" s="18" t="s">
         <v>172</v>
       </c>
       <c r="D20" s="5" t="s">
@@ -1895,8 +1895,8 @@
     </row>
     <row r="21" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A21" s="5"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="11"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="18"/>
       <c r="D21" s="5" t="s">
         <v>202</v>
       </c>
@@ -1912,8 +1912,8 @@
     </row>
     <row r="22" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A22" s="5"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="11"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="18"/>
       <c r="D22" s="5" t="s">
         <v>203</v>
       </c>
@@ -1929,8 +1929,8 @@
     </row>
     <row r="23" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A23" s="5"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="11"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="18"/>
       <c r="D23" s="5" t="s">
         <v>204</v>
       </c>
@@ -1946,14 +1946,14 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24" s="5"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="10" t="s">
+      <c r="B24" s="12"/>
+      <c r="C24" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="E24" s="12" t="str">
+      <c r="E24" s="11" t="str">
         <f t="shared" si="1"/>
         <v>Foreservation.jsp</v>
       </c>
@@ -1965,10 +1965,10 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25" s="5"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="13"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="12"/>
       <c r="F25" s="3" t="s">
         <v>168</v>
       </c>
@@ -1977,10 +1977,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26" s="5"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="13"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="12"/>
       <c r="F26" s="3" t="s">
         <v>170</v>
       </c>
@@ -1989,10 +1989,10 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" s="5"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="13"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="12"/>
       <c r="F27" s="3" t="s">
         <v>171</v>
       </c>
@@ -2001,10 +2001,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A28" s="5"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="14"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="13"/>
       <c r="F28" s="3" t="s">
         <v>172</v>
       </c>
@@ -2013,14 +2013,14 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29" s="5"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="10" t="s">
+      <c r="B29" s="12"/>
+      <c r="C29" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D29" s="14" t="s">
         <v>211</v>
       </c>
-      <c r="E29" s="12" t="str">
+      <c r="E29" s="11" t="str">
         <f t="shared" si="1"/>
         <v>GnrSrch.jsp</v>
       </c>
@@ -2032,10 +2032,10 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30" s="5"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="13"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="12"/>
       <c r="F30" s="3" t="s">
         <v>187</v>
       </c>
@@ -2044,10 +2044,10 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A31" s="5"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="13"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="12"/>
       <c r="F31" s="3" t="s">
         <v>189</v>
       </c>
@@ -2056,10 +2056,10 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A32" s="5"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="13"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="12"/>
       <c r="F32" s="3" t="s">
         <v>190</v>
       </c>
@@ -2068,10 +2068,10 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A33" s="5"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="13"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="12"/>
       <c r="F33" s="8" t="s">
         <v>194</v>
       </c>
@@ -2080,10 +2080,10 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A34" s="5"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="14"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="13"/>
       <c r="F34" s="3" t="s">
         <v>188</v>
       </c>
@@ -2092,14 +2092,14 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A35" s="5"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="10" t="s">
+      <c r="B35" s="12"/>
+      <c r="C35" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="D35" s="14" t="s">
         <v>213</v>
       </c>
-      <c r="E35" s="12" t="str">
+      <c r="E35" s="11" t="str">
         <f t="shared" si="1"/>
         <v>MonthSrch.jsp</v>
       </c>
@@ -2111,10 +2111,10 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A36" s="5"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="13"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="12"/>
       <c r="F36" s="3" t="s">
         <v>187</v>
       </c>
@@ -2123,10 +2123,10 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A37" s="5"/>
-      <c r="B37" s="13"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="14"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="13"/>
       <c r="F37" s="3" t="s">
         <v>195</v>
       </c>
@@ -2137,14 +2137,14 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A38" s="5"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="10" t="s">
+      <c r="B38" s="12"/>
+      <c r="C38" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="D38" s="10" t="s">
+      <c r="D38" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="E38" s="12" t="str">
+      <c r="E38" s="11" t="str">
         <f t="shared" si="1"/>
         <v>GnrResrv.jsp</v>
       </c>
@@ -2156,10 +2156,10 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A39" s="5"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="13"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="12"/>
       <c r="F39" s="3" t="s">
         <v>214</v>
       </c>
@@ -2168,10 +2168,10 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A40" s="5"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="13"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="12"/>
       <c r="F40" s="3" t="s">
         <v>215</v>
       </c>
@@ -2180,10 +2180,10 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A41" s="5"/>
-      <c r="B41" s="13"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="13"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="12"/>
       <c r="F41" s="3" t="s">
         <v>216</v>
       </c>
@@ -2192,10 +2192,10 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A42" s="5"/>
-      <c r="B42" s="13"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="13"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="12"/>
       <c r="F42" s="8" t="s">
         <v>217</v>
       </c>
@@ -2204,10 +2204,10 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A43" s="5"/>
-      <c r="B43" s="13"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="14"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="13"/>
       <c r="F43" s="3" t="s">
         <v>189</v>
       </c>
@@ -2218,14 +2218,14 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A44" s="5"/>
-      <c r="B44" s="13"/>
-      <c r="C44" s="10" t="s">
+      <c r="B44" s="12"/>
+      <c r="C44" s="14" t="s">
         <v>210</v>
       </c>
-      <c r="D44" s="10" t="s">
+      <c r="D44" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="E44" s="12" t="str">
+      <c r="E44" s="11" t="str">
         <f t="shared" si="1"/>
         <v>PrgmSrch.jsp</v>
       </c>
@@ -2237,10 +2237,10 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A45" s="5"/>
-      <c r="B45" s="13"/>
-      <c r="C45" s="10"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="13"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="12"/>
       <c r="F45" s="3" t="s">
         <v>187</v>
       </c>
@@ -2249,10 +2249,10 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A46" s="5"/>
-      <c r="B46" s="13"/>
-      <c r="C46" s="10"/>
-      <c r="D46" s="10"/>
-      <c r="E46" s="13"/>
+      <c r="B46" s="12"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="12"/>
       <c r="F46" s="3" t="s">
         <v>189</v>
       </c>
@@ -2261,10 +2261,10 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A47" s="5"/>
-      <c r="B47" s="13"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="10"/>
-      <c r="E47" s="13"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="12"/>
       <c r="F47" s="3" t="s">
         <v>190</v>
       </c>
@@ -2273,10 +2273,10 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A48" s="5"/>
-      <c r="B48" s="13"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="14"/>
+      <c r="B48" s="12"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="13"/>
       <c r="F48" s="8" t="s">
         <v>193</v>
       </c>
@@ -2285,14 +2285,14 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A49" s="5"/>
-      <c r="B49" s="13"/>
-      <c r="C49" s="10" t="s">
+      <c r="B49" s="12"/>
+      <c r="C49" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D49" s="10" t="s">
+      <c r="D49" s="14" t="s">
         <v>192</v>
       </c>
-      <c r="E49" s="12" t="str">
+      <c r="E49" s="11" t="str">
         <f t="shared" si="1"/>
         <v>PrgmResrv.jsp</v>
       </c>
@@ -2304,10 +2304,10 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A50" s="5"/>
-      <c r="B50" s="13"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="13"/>
+      <c r="B50" s="12"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="12"/>
       <c r="F50" s="3" t="s">
         <v>218</v>
       </c>
@@ -2316,10 +2316,10 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A51" s="5"/>
-      <c r="B51" s="13"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
-      <c r="E51" s="13"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="12"/>
       <c r="F51" s="3" t="s">
         <v>219</v>
       </c>
@@ -2328,10 +2328,10 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A52" s="5"/>
-      <c r="B52" s="13"/>
-      <c r="C52" s="10"/>
-      <c r="D52" s="10"/>
-      <c r="E52" s="13"/>
+      <c r="B52" s="12"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="12"/>
       <c r="F52" s="3" t="s">
         <v>221</v>
       </c>
@@ -2340,10 +2340,10 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A53" s="5"/>
-      <c r="B53" s="13"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="10"/>
-      <c r="E53" s="14"/>
+      <c r="B53" s="12"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="13"/>
       <c r="F53" s="3" t="s">
         <v>189</v>
       </c>
@@ -2354,14 +2354,14 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A54" s="5"/>
-      <c r="B54" s="13"/>
-      <c r="C54" s="10" t="s">
+      <c r="B54" s="12"/>
+      <c r="C54" s="14" t="s">
         <v>222</v>
       </c>
-      <c r="D54" s="10" t="s">
+      <c r="D54" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="E54" s="12" t="str">
+      <c r="E54" s="11" t="str">
         <f t="shared" si="1"/>
         <v>PayInfo.jsp</v>
       </c>
@@ -2373,10 +2373,10 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A55" s="5"/>
-      <c r="B55" s="13"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
-      <c r="E55" s="13"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="14"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="12"/>
       <c r="F55" s="3" t="s">
         <v>226</v>
       </c>
@@ -2385,10 +2385,10 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A56" s="5"/>
-      <c r="B56" s="13"/>
-      <c r="C56" s="10"/>
-      <c r="D56" s="10"/>
-      <c r="E56" s="13"/>
+      <c r="B56" s="12"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="12"/>
       <c r="F56" s="3" t="s">
         <v>227</v>
       </c>
@@ -2397,10 +2397,10 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A57" s="5"/>
-      <c r="B57" s="13"/>
-      <c r="C57" s="10"/>
-      <c r="D57" s="10"/>
-      <c r="E57" s="13"/>
+      <c r="B57" s="12"/>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="12"/>
       <c r="F57" s="3" t="s">
         <v>228</v>
       </c>
@@ -2409,10 +2409,10 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A58" s="5"/>
-      <c r="B58" s="13"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="10"/>
-      <c r="E58" s="14"/>
+      <c r="B58" s="12"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="13"/>
       <c r="F58" s="3" t="s">
         <v>229</v>
       </c>
@@ -2421,7 +2421,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A59" s="5"/>
-      <c r="B59" s="13"/>
+      <c r="B59" s="12"/>
       <c r="C59" s="1" t="s">
         <v>231</v>
       </c>
@@ -2440,14 +2440,14 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A60" s="5"/>
-      <c r="B60" s="13"/>
-      <c r="C60" s="10" t="s">
+      <c r="B60" s="12"/>
+      <c r="C60" s="14" t="s">
         <v>228</v>
       </c>
-      <c r="D60" s="10" t="s">
+      <c r="D60" s="14" t="s">
         <v>236</v>
       </c>
-      <c r="E60" s="12" t="str">
+      <c r="E60" s="11" t="str">
         <f t="shared" si="1"/>
         <v>Mypage.jsp</v>
       </c>
@@ -2459,10 +2459,10 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A61" s="5"/>
-      <c r="B61" s="13"/>
-      <c r="C61" s="10"/>
-      <c r="D61" s="10"/>
-      <c r="E61" s="13"/>
+      <c r="B61" s="12"/>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="12"/>
       <c r="F61" s="3" t="s">
         <v>238</v>
       </c>
@@ -2471,10 +2471,10 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A62" s="5"/>
-      <c r="B62" s="13"/>
-      <c r="C62" s="10"/>
-      <c r="D62" s="10"/>
-      <c r="E62" s="13"/>
+      <c r="B62" s="12"/>
+      <c r="C62" s="14"/>
+      <c r="D62" s="14"/>
+      <c r="E62" s="12"/>
       <c r="F62" s="3" t="s">
         <v>239</v>
       </c>
@@ -2483,10 +2483,10 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A63" s="5"/>
-      <c r="B63" s="13"/>
-      <c r="C63" s="10"/>
-      <c r="D63" s="10"/>
-      <c r="E63" s="13"/>
+      <c r="B63" s="12"/>
+      <c r="C63" s="14"/>
+      <c r="D63" s="14"/>
+      <c r="E63" s="12"/>
       <c r="F63" s="3" t="s">
         <v>240</v>
       </c>
@@ -2495,10 +2495,10 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A64" s="5"/>
-      <c r="B64" s="13"/>
-      <c r="C64" s="10"/>
-      <c r="D64" s="10"/>
-      <c r="E64" s="14"/>
+      <c r="B64" s="12"/>
+      <c r="C64" s="14"/>
+      <c r="D64" s="14"/>
+      <c r="E64" s="13"/>
       <c r="F64" s="3" t="s">
         <v>241</v>
       </c>
@@ -2507,14 +2507,14 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A65" s="5"/>
-      <c r="B65" s="13"/>
-      <c r="C65" s="10" t="s">
+      <c r="B65" s="12"/>
+      <c r="C65" s="14" t="s">
         <v>237</v>
       </c>
-      <c r="D65" s="10" t="s">
+      <c r="D65" s="14" t="s">
         <v>242</v>
       </c>
-      <c r="E65" s="12" t="str">
+      <c r="E65" s="11" t="str">
         <f t="shared" si="1"/>
         <v>MyResrv.jsp</v>
       </c>
@@ -2526,10 +2526,10 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A66" s="5"/>
-      <c r="B66" s="13"/>
-      <c r="C66" s="10"/>
-      <c r="D66" s="10"/>
-      <c r="E66" s="13"/>
+      <c r="B66" s="12"/>
+      <c r="C66" s="14"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="12"/>
       <c r="F66" s="3" t="s">
         <v>227</v>
       </c>
@@ -2538,10 +2538,10 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A67" s="5"/>
-      <c r="B67" s="13"/>
-      <c r="C67" s="10"/>
-      <c r="D67" s="10"/>
-      <c r="E67" s="13"/>
+      <c r="B67" s="12"/>
+      <c r="C67" s="14"/>
+      <c r="D67" s="14"/>
+      <c r="E67" s="12"/>
       <c r="F67" s="3" t="s">
         <v>229</v>
       </c>
@@ -2550,10 +2550,10 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A68" s="5"/>
-      <c r="B68" s="13"/>
-      <c r="C68" s="10"/>
-      <c r="D68" s="10"/>
-      <c r="E68" s="14"/>
+      <c r="B68" s="12"/>
+      <c r="C68" s="14"/>
+      <c r="D68" s="14"/>
+      <c r="E68" s="13"/>
       <c r="F68" s="3" t="s">
         <v>244</v>
       </c>
@@ -2562,14 +2562,14 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A69" s="5"/>
-      <c r="B69" s="13"/>
-      <c r="C69" s="10" t="s">
+      <c r="B69" s="12"/>
+      <c r="C69" s="14" t="s">
         <v>229</v>
       </c>
-      <c r="D69" s="10" t="s">
+      <c r="D69" s="14" t="s">
         <v>246</v>
       </c>
-      <c r="E69" s="12" t="str">
+      <c r="E69" s="11" t="str">
         <f t="shared" si="1"/>
         <v>ResrvCancle.jsp</v>
       </c>
@@ -2581,10 +2581,10 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A70" s="5"/>
-      <c r="B70" s="13"/>
-      <c r="C70" s="10"/>
-      <c r="D70" s="10"/>
-      <c r="E70" s="14"/>
+      <c r="B70" s="12"/>
+      <c r="C70" s="14"/>
+      <c r="D70" s="14"/>
+      <c r="E70" s="13"/>
       <c r="F70" s="3" t="s">
         <v>248</v>
       </c>
@@ -2593,14 +2593,14 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A71" s="5"/>
-      <c r="B71" s="13"/>
-      <c r="C71" s="10" t="s">
+      <c r="B71" s="12"/>
+      <c r="C71" s="14" t="s">
         <v>249</v>
       </c>
-      <c r="D71" s="10" t="s">
+      <c r="D71" s="14" t="s">
         <v>254</v>
       </c>
-      <c r="E71" s="12" t="str">
+      <c r="E71" s="11" t="str">
         <f t="shared" ref="E71:E85" si="2">D71&amp;".jsp"</f>
         <v>ResrvInfo.jsp</v>
       </c>
@@ -2612,10 +2612,10 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A72" s="5"/>
-      <c r="B72" s="13"/>
-      <c r="C72" s="10"/>
-      <c r="D72" s="10"/>
-      <c r="E72" s="13"/>
+      <c r="B72" s="12"/>
+      <c r="C72" s="14"/>
+      <c r="D72" s="14"/>
+      <c r="E72" s="12"/>
       <c r="F72" s="3" t="s">
         <v>250</v>
       </c>
@@ -2624,10 +2624,10 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A73" s="5"/>
-      <c r="B73" s="13"/>
-      <c r="C73" s="10"/>
-      <c r="D73" s="10"/>
-      <c r="E73" s="13"/>
+      <c r="B73" s="12"/>
+      <c r="C73" s="14"/>
+      <c r="D73" s="14"/>
+      <c r="E73" s="12"/>
       <c r="F73" s="3" t="s">
         <v>253</v>
       </c>
@@ -2636,10 +2636,10 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A74" s="5"/>
-      <c r="B74" s="13"/>
-      <c r="C74" s="10"/>
-      <c r="D74" s="10"/>
-      <c r="E74" s="14"/>
+      <c r="B74" s="12"/>
+      <c r="C74" s="14"/>
+      <c r="D74" s="14"/>
+      <c r="E74" s="13"/>
       <c r="F74" s="3" t="s">
         <v>252</v>
       </c>
@@ -2648,7 +2648,7 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A75" s="5"/>
-      <c r="B75" s="13"/>
+      <c r="B75" s="12"/>
       <c r="C75" s="1" t="s">
         <v>238</v>
       </c>
@@ -2667,14 +2667,14 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A76" s="5"/>
-      <c r="B76" s="13"/>
-      <c r="C76" s="10" t="s">
+      <c r="B76" s="12"/>
+      <c r="C76" s="14" t="s">
         <v>257</v>
       </c>
-      <c r="D76" s="10" t="s">
+      <c r="D76" s="14" t="s">
         <v>258</v>
       </c>
-      <c r="E76" s="12" t="str">
+      <c r="E76" s="11" t="str">
         <f t="shared" si="2"/>
         <v>MyQnalist.jsp</v>
       </c>
@@ -2686,10 +2686,10 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A77" s="5"/>
-      <c r="B77" s="13"/>
-      <c r="C77" s="10"/>
-      <c r="D77" s="10"/>
-      <c r="E77" s="13"/>
+      <c r="B77" s="12"/>
+      <c r="C77" s="14"/>
+      <c r="D77" s="14"/>
+      <c r="E77" s="12"/>
       <c r="F77" s="3" t="s">
         <v>259</v>
       </c>
@@ -2698,10 +2698,10 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A78" s="5"/>
-      <c r="B78" s="13"/>
-      <c r="C78" s="10"/>
-      <c r="D78" s="10"/>
-      <c r="E78" s="14"/>
+      <c r="B78" s="12"/>
+      <c r="C78" s="14"/>
+      <c r="D78" s="14"/>
+      <c r="E78" s="13"/>
       <c r="F78" s="3" t="s">
         <v>260</v>
       </c>
@@ -2710,14 +2710,14 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A79" s="5"/>
-      <c r="B79" s="13"/>
-      <c r="C79" s="10" t="s">
+      <c r="B79" s="12"/>
+      <c r="C79" s="14" t="s">
         <v>261</v>
       </c>
-      <c r="D79" s="10" t="s">
+      <c r="D79" s="14" t="s">
         <v>262</v>
       </c>
-      <c r="E79" s="12" t="str">
+      <c r="E79" s="11" t="str">
         <f t="shared" si="2"/>
         <v>QnaReg.jsp</v>
       </c>
@@ -2729,10 +2729,10 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A80" s="5"/>
-      <c r="B80" s="13"/>
-      <c r="C80" s="10"/>
-      <c r="D80" s="10"/>
-      <c r="E80" s="14"/>
+      <c r="B80" s="12"/>
+      <c r="C80" s="14"/>
+      <c r="D80" s="14"/>
+      <c r="E80" s="13"/>
       <c r="F80" s="3" t="s">
         <v>248</v>
       </c>
@@ -2741,7 +2741,7 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A81" s="5"/>
-      <c r="B81" s="13"/>
+      <c r="B81" s="12"/>
       <c r="C81" s="1" t="s">
         <v>240</v>
       </c>
@@ -2760,14 +2760,14 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A82" s="5"/>
-      <c r="B82" s="13"/>
-      <c r="C82" s="10" t="s">
+      <c r="B82" s="12"/>
+      <c r="C82" s="14" t="s">
         <v>265</v>
       </c>
-      <c r="D82" s="10" t="s">
+      <c r="D82" s="14" t="s">
         <v>266</v>
       </c>
-      <c r="E82" s="12" t="str">
+      <c r="E82" s="11" t="str">
         <f t="shared" si="2"/>
         <v>MyInfoEdit.jsp</v>
       </c>
@@ -2779,10 +2779,10 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A83" s="5"/>
-      <c r="B83" s="13"/>
-      <c r="C83" s="10"/>
-      <c r="D83" s="10"/>
-      <c r="E83" s="13"/>
+      <c r="B83" s="12"/>
+      <c r="C83" s="14"/>
+      <c r="D83" s="14"/>
+      <c r="E83" s="12"/>
       <c r="F83" s="3" t="s">
         <v>268</v>
       </c>
@@ -2791,10 +2791,10 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A84" s="5"/>
-      <c r="B84" s="13"/>
-      <c r="C84" s="10"/>
-      <c r="D84" s="10"/>
-      <c r="E84" s="14"/>
+      <c r="B84" s="12"/>
+      <c r="C84" s="14"/>
+      <c r="D84" s="14"/>
+      <c r="E84" s="13"/>
       <c r="F84" s="3" t="s">
         <v>269</v>
       </c>
@@ -2803,7 +2803,7 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A85" s="5"/>
-      <c r="B85" s="14"/>
+      <c r="B85" s="13"/>
       <c r="C85" s="1" t="s">
         <v>241</v>
       </c>
@@ -2822,15 +2822,32 @@
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="E76:E78"/>
-    <mergeCell ref="E79:E80"/>
-    <mergeCell ref="E82:E84"/>
-    <mergeCell ref="E49:E53"/>
-    <mergeCell ref="E54:E58"/>
-    <mergeCell ref="E60:E64"/>
-    <mergeCell ref="E65:E68"/>
-    <mergeCell ref="E69:E70"/>
-    <mergeCell ref="E71:E74"/>
+    <mergeCell ref="D38:D43"/>
+    <mergeCell ref="C38:C43"/>
+    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="D69:D70"/>
+    <mergeCell ref="D44:D48"/>
+    <mergeCell ref="C54:C58"/>
+    <mergeCell ref="D54:D58"/>
+    <mergeCell ref="D49:D53"/>
+    <mergeCell ref="C49:C53"/>
+    <mergeCell ref="C44:C48"/>
+    <mergeCell ref="C2:C7"/>
+    <mergeCell ref="D60:D64"/>
+    <mergeCell ref="C60:C64"/>
+    <mergeCell ref="D65:D68"/>
+    <mergeCell ref="C65:C68"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="D35:D37"/>
+    <mergeCell ref="C15:C19"/>
+    <mergeCell ref="D15:D19"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="C29:C34"/>
+    <mergeCell ref="D29:D34"/>
+    <mergeCell ref="D24:D28"/>
+    <mergeCell ref="C24:C28"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="C9:C11"/>
     <mergeCell ref="D82:D84"/>
     <mergeCell ref="C82:C84"/>
     <mergeCell ref="B2:B85"/>
@@ -2847,32 +2864,15 @@
     <mergeCell ref="C76:C78"/>
     <mergeCell ref="D79:D80"/>
     <mergeCell ref="C79:C80"/>
-    <mergeCell ref="C2:C7"/>
-    <mergeCell ref="D60:D64"/>
-    <mergeCell ref="C60:C64"/>
-    <mergeCell ref="D65:D68"/>
-    <mergeCell ref="C65:C68"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="D35:D37"/>
-    <mergeCell ref="C15:C19"/>
-    <mergeCell ref="D15:D19"/>
-    <mergeCell ref="C20:C23"/>
-    <mergeCell ref="C29:C34"/>
-    <mergeCell ref="D29:D34"/>
-    <mergeCell ref="D24:D28"/>
-    <mergeCell ref="C24:C28"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="D38:D43"/>
-    <mergeCell ref="C38:C43"/>
-    <mergeCell ref="C69:C70"/>
-    <mergeCell ref="D69:D70"/>
-    <mergeCell ref="D44:D48"/>
-    <mergeCell ref="C54:C58"/>
-    <mergeCell ref="D54:D58"/>
-    <mergeCell ref="D49:D53"/>
-    <mergeCell ref="C49:C53"/>
-    <mergeCell ref="C44:C48"/>
+    <mergeCell ref="E76:E78"/>
+    <mergeCell ref="E79:E80"/>
+    <mergeCell ref="E82:E84"/>
+    <mergeCell ref="E49:E53"/>
+    <mergeCell ref="E54:E58"/>
+    <mergeCell ref="E60:E64"/>
+    <mergeCell ref="E65:E68"/>
+    <mergeCell ref="E69:E70"/>
+    <mergeCell ref="E71:E74"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
edit nav and add Jimlist
</commit_message>
<xml_diff>
--- a/document/Foreservation_ViewList.xlsx
+++ b/document/Foreservation_ViewList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github_Intern2019\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20578079-BAE1-4C97-8BC3-70C8B14B3862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6180E1A9-B3D7-4826-A0B4-DF0BAB270B42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="297">
   <si>
     <t>OBJECT</t>
   </si>
@@ -871,10 +871,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>MyQnalist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>글쓰기</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -919,10 +915,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>MyWidrw</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>사용자</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1022,6 +1014,40 @@
   </si>
   <si>
     <t>2024.03.15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>예약정보</t>
+  </si>
+  <si>
+    <t>나의정보</t>
+  </si>
+  <si>
+    <t>NavMyResrv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NavJimList</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qnalist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NavQnaList</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NavMyInfo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NavWidrw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Widrw</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1117,7 +1143,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1149,13 +1175,16 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1499,8 +1528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DF753CA-3B43-42CB-99AB-2EC6963C2F06}">
   <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23:E26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.2" x14ac:dyDescent="0.45"/>
@@ -1517,22 +1546,22 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>167</v>
@@ -1543,31 +1572,31 @@
     </row>
     <row r="2" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="5"/>
-      <c r="B2" s="12" t="s">
-        <v>264</v>
-      </c>
-      <c r="C2" s="12" t="s">
+      <c r="B2" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>174</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E2" s="10" t="str">
         <f>D2&amp;".jsp"</f>
         <v>NavMain.jsp</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
       <c r="D3" s="5" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E3" s="5" t="str">
         <f>D3&amp;".jsp"</f>
@@ -1581,27 +1610,27 @@
     </row>
     <row r="4" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="5"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
       <c r="D4" s="5" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E4" s="10" t="str">
         <f t="shared" ref="E4" si="0">D4&amp;".jsp"</f>
         <v>NavSiteInfo.jsp</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" s="5"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
       <c r="D5" s="5" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E5" s="10" t="str">
         <f>D5&amp;".jsp"</f>
@@ -1615,256 +1644,281 @@
     </row>
     <row r="6" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A6" s="5"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
       <c r="D6" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E6" s="10" t="str">
         <f>D6&amp;".jsp"</f>
         <v>NavPrgmInfo.jsp</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A7" s="5"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
       <c r="D7" s="5" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E7" s="10" t="str">
-        <f t="shared" ref="E7:E85" si="1">D7&amp;".jsp"</f>
+        <f>D7&amp;".jsp"</f>
         <v>NavMypage.jsp</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>224</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A8" s="5"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="5" t="s">
-        <v>173</v>
-      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
       <c r="D8" s="5" t="s">
-        <v>273</v>
+        <v>290</v>
       </c>
       <c r="E8" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>Footer.jsp</v>
-      </c>
-      <c r="F8" s="9"/>
+        <f t="shared" ref="E8:E12" si="1">D8&amp;".jsp"</f>
+        <v>NavMyResrv.jsp</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>288</v>
+      </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A9" s="5"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12" t="s">
-        <v>275</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>180</v>
-      </c>
-      <c r="E9" s="13" t="str">
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="E9" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>ForeservationInfo.jsp</v>
+        <v>NavJimList.jsp</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>230</v>
+        <v>281</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A10" s="5"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="13"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="E10" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v>NavQnaList.jsp</v>
+      </c>
       <c r="F10" s="9" t="s">
-        <v>271</v>
+        <v>250</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A11" s="5"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="13"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="E11" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v>NavMyInfo.jsp</v>
+      </c>
       <c r="F11" s="9" t="s">
-        <v>231</v>
+        <v>289</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A12" s="5"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="13"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="E12" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v>NavWidrw.jsp</v>
+      </c>
       <c r="F12" s="9" t="s">
-        <v>272</v>
+        <v>235</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A13" s="5"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="9" t="s">
-        <v>224</v>
-      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="E13" s="10" t="str">
+        <f t="shared" ref="E13:E85" si="2">D13&amp;".jsp"</f>
+        <v>Footer.jsp</v>
+      </c>
+      <c r="F13" s="9"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A14" s="5"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="13"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="E14" s="13" t="str">
+        <f t="shared" si="2"/>
+        <v>ForeservationInfo.jsp</v>
+      </c>
       <c r="F14" s="9" t="s">
-        <v>170</v>
+        <v>230</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A15" s="5"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="E15" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>SiteInfo.jsp</v>
-      </c>
-      <c r="F15" s="9"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="9" t="s">
+        <v>269</v>
+      </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A16" s="5"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="E16" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>RoomInfo.jsp</v>
-      </c>
-      <c r="F16" s="9"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="9" t="s">
+        <v>231</v>
+      </c>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A17" s="5"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="E17" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>PrgmInfo.jsp</v>
-      </c>
-      <c r="F17" s="9"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="9" t="s">
+        <v>270</v>
+      </c>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
     </row>
     <row r="18" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A18" s="5"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="11" t="s">
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="9" t="s">
-        <v>232</v>
-      </c>
-      <c r="G18" s="5"/>
+      <c r="G18" s="5" t="s">
+        <v>285</v>
+      </c>
       <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A19" s="5"/>
-      <c r="B19" s="12"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
-      <c r="E19" s="12"/>
+      <c r="E19" s="13"/>
       <c r="F19" s="9" t="s">
-        <v>283</v>
+        <v>170</v>
       </c>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A20" s="5"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="9" t="s">
-        <v>250</v>
-      </c>
+      <c r="B20" s="11"/>
+      <c r="C20" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="E20" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>SiteInfo.jsp</v>
+      </c>
+      <c r="F20" s="9"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A21" s="5"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="9" t="s">
-        <v>234</v>
-      </c>
+      <c r="B21" s="11"/>
+      <c r="C21" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="E21" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>RoomInfo.jsp</v>
+      </c>
+      <c r="F21" s="9"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A22" s="5"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="9" t="s">
-        <v>235</v>
-      </c>
+      <c r="B22" s="11"/>
+      <c r="C22" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="E22" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>PrgmInfo.jsp</v>
+      </c>
+      <c r="F22" s="9"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23" s="5"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="11" t="s">
+      <c r="B23" s="11"/>
+      <c r="C23" s="12" t="s">
         <v>232</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="12" t="s">
         <v>236</v>
       </c>
       <c r="E23" s="13" t="str">
@@ -1876,61 +1930,61 @@
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24" s="5"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
       <c r="E24" s="13"/>
       <c r="F24" s="3" t="s">
         <v>223</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25" s="5"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
       <c r="E25" s="13"/>
       <c r="F25" s="3" t="s">
         <v>225</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26" s="5"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
       <c r="E26" s="13"/>
       <c r="F26" s="3" t="s">
         <v>238</v>
       </c>
       <c r="G26" s="3"/>
       <c r="H26" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" s="5"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="11" t="s">
+      <c r="B27" s="11"/>
+      <c r="C27" s="12" t="s">
         <v>225</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D27" s="12" t="s">
         <v>240</v>
       </c>
-      <c r="E27" s="12" t="str">
+      <c r="E27" s="11" t="str">
         <f>D27&amp;".jsp"</f>
         <v>ResrvCancle.jsp</v>
       </c>
@@ -1942,10 +1996,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A28" s="5"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="12"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="11"/>
       <c r="F28" s="3" t="s">
         <v>242</v>
       </c>
@@ -1954,15 +2008,15 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29" s="5"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="11" t="s">
+      <c r="B29" s="11"/>
+      <c r="C29" s="12" t="s">
         <v>238</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D29" s="12" t="s">
         <v>247</v>
       </c>
-      <c r="E29" s="12" t="str">
-        <f t="shared" ref="E29:E43" si="2">D29&amp;".jsp"</f>
+      <c r="E29" s="11" t="str">
+        <f t="shared" ref="E29:E43" si="3">D29&amp;".jsp"</f>
         <v>ResrvInfo.jsp</v>
       </c>
       <c r="F29" s="3" t="s">
@@ -1973,10 +2027,10 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30" s="5"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="12"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="11"/>
       <c r="F30" s="3" t="s">
         <v>243</v>
       </c>
@@ -1985,10 +2039,10 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A31" s="5"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="12"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="11"/>
       <c r="F31" s="3" t="s">
         <v>246</v>
       </c>
@@ -1997,10 +2051,10 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A32" s="5"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="12"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="11"/>
       <c r="F32" s="3" t="s">
         <v>245</v>
       </c>
@@ -2009,7 +2063,7 @@
     </row>
     <row r="33" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A33" s="5"/>
-      <c r="B33" s="12"/>
+      <c r="B33" s="11"/>
       <c r="C33" s="1" t="s">
         <v>233</v>
       </c>
@@ -2017,7 +2071,7 @@
         <v>248</v>
       </c>
       <c r="E33" s="5" t="str">
-        <f t="shared" ref="E33" si="3">D33&amp;".jsp"</f>
+        <f t="shared" ref="E33" si="4">D33&amp;".jsp"</f>
         <v>JimList.jsp</v>
       </c>
       <c r="F33" s="3" t="s">
@@ -2025,83 +2079,83 @@
       </c>
       <c r="G33" s="5"/>
       <c r="H33" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A34" s="5"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="11" t="s">
+      <c r="B34" s="11"/>
+      <c r="C34" s="12" t="s">
         <v>250</v>
       </c>
-      <c r="D34" s="11" t="s">
-        <v>251</v>
-      </c>
-      <c r="E34" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v>MyQnalist.jsp</v>
+      <c r="D34" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="E34" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>Qnalist.jsp</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>182</v>
       </c>
       <c r="G34" s="3"/>
       <c r="H34" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A35" s="5"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="12"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="11"/>
       <c r="F35" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G35" s="3"/>
       <c r="H35" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A36" s="5"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="12"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="11"/>
       <c r="F36" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G36" s="3"/>
       <c r="H36" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A37" s="5"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="11" t="s">
+      <c r="B37" s="11"/>
+      <c r="C37" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="D37" s="12" t="s">
         <v>254</v>
       </c>
-      <c r="D37" s="11" t="s">
+      <c r="E37" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>QnaReg.jsp</v>
+      </c>
+      <c r="F37" s="3" t="s">
         <v>255</v>
-      </c>
-      <c r="E37" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v>QnaReg.jsp</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>256</v>
       </c>
       <c r="G37" s="3"/>
       <c r="H37" s="1"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A38" s="5"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="12"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="11"/>
       <c r="F38" s="3" t="s">
         <v>242</v>
       </c>
@@ -2110,15 +2164,15 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A39" s="5"/>
-      <c r="B39" s="12"/>
+      <c r="B39" s="11"/>
       <c r="C39" s="1" t="s">
         <v>234</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E39" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>MyInfo.jsp</v>
       </c>
       <c r="F39" s="3" t="s">
@@ -2126,84 +2180,84 @@
       </c>
       <c r="G39" s="3"/>
       <c r="H39" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A40" s="5"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="11" t="s">
+      <c r="B40" s="11"/>
+      <c r="C40" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="D40" s="12" t="s">
         <v>258</v>
       </c>
-      <c r="D40" s="11" t="s">
+      <c r="E40" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>MyInfoEdit.jsp</v>
+      </c>
+      <c r="F40" s="3" t="s">
         <v>259</v>
-      </c>
-      <c r="E40" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v>MyInfoEdit.jsp</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>260</v>
       </c>
       <c r="G40" s="3"/>
       <c r="H40" s="1"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A41" s="5"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="12"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="11"/>
       <c r="F41" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G41" s="3"/>
       <c r="H41" s="1"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A42" s="5"/>
-      <c r="B42" s="12"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="12"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="11"/>
       <c r="F42" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G42" s="3"/>
       <c r="H42" s="1"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A43" s="5"/>
-      <c r="B43" s="12"/>
+      <c r="B43" s="11"/>
       <c r="C43" s="1" t="s">
         <v>235</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>263</v>
+        <v>296</v>
       </c>
       <c r="E43" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>MyWidrw.jsp</v>
+        <f t="shared" si="3"/>
+        <v>Widrw.jsp</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>235</v>
       </c>
       <c r="G43" s="3"/>
       <c r="H43" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="44" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A44" s="5"/>
-      <c r="B44" s="12"/>
-      <c r="C44" s="12" t="s">
+      <c r="B44" s="11"/>
+      <c r="C44" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="D44" s="12" t="s">
+      <c r="D44" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="E44" s="12" t="str">
-        <f t="shared" si="1"/>
+      <c r="E44" s="11" t="str">
+        <f t="shared" si="2"/>
         <v>Login.jsp</v>
       </c>
       <c r="F44" s="9" t="s">
@@ -2214,10 +2268,10 @@
     </row>
     <row r="45" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A45" s="5"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
       <c r="F45" s="9" t="s">
         <v>193</v>
       </c>
@@ -2226,10 +2280,10 @@
     </row>
     <row r="46" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A46" s="5"/>
-      <c r="B46" s="12"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="12"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
       <c r="F46" s="9" t="s">
         <v>194</v>
       </c>
@@ -2238,10 +2292,10 @@
     </row>
     <row r="47" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A47" s="5"/>
-      <c r="B47" s="12"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="12"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
       <c r="F47" s="9" t="s">
         <v>195</v>
       </c>
@@ -2250,10 +2304,10 @@
     </row>
     <row r="48" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A48" s="5"/>
-      <c r="B48" s="12"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="12"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
       <c r="F48" s="9" t="s">
         <v>196</v>
       </c>
@@ -2262,15 +2316,15 @@
     </row>
     <row r="49" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A49" s="5"/>
-      <c r="B49" s="12"/>
-      <c r="C49" s="12" t="s">
+      <c r="B49" s="11"/>
+      <c r="C49" s="11" t="s">
         <v>171</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>197</v>
       </c>
       <c r="E49" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Acnt_RegAgr.jsp</v>
       </c>
       <c r="F49" s="9" t="s">
@@ -2281,13 +2335,13 @@
     </row>
     <row r="50" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A50" s="5"/>
-      <c r="B50" s="12"/>
-      <c r="C50" s="12"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
       <c r="D50" s="5" t="s">
         <v>198</v>
       </c>
       <c r="E50" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Acnt_RegChk.jsp</v>
       </c>
       <c r="F50" s="9" t="s">
@@ -2298,13 +2352,13 @@
     </row>
     <row r="51" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A51" s="5"/>
-      <c r="B51" s="12"/>
-      <c r="C51" s="12"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
       <c r="D51" s="5" t="s">
         <v>199</v>
       </c>
       <c r="E51" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Acnt_RegInfo.jsp</v>
       </c>
       <c r="F51" s="9" t="s">
@@ -2315,13 +2369,13 @@
     </row>
     <row r="52" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A52" s="5"/>
-      <c r="B52" s="12"/>
-      <c r="C52" s="12"/>
+      <c r="B52" s="11"/>
+      <c r="C52" s="11"/>
       <c r="D52" s="5" t="s">
         <v>200</v>
       </c>
       <c r="E52" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Acnt_RegCom.jsp</v>
       </c>
       <c r="F52" s="9" t="s">
@@ -2332,15 +2386,15 @@
     </row>
     <row r="53" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A53" s="5"/>
-      <c r="B53" s="12"/>
+      <c r="B53" s="11"/>
       <c r="C53" s="5" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E53" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>FindID.jsp</v>
       </c>
       <c r="F53" s="9"/>
@@ -2349,15 +2403,15 @@
     </row>
     <row r="54" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A54" s="5"/>
-      <c r="B54" s="12"/>
+      <c r="B54" s="11"/>
       <c r="C54" s="5" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E54" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>FindPw.jsp</v>
       </c>
       <c r="F54" s="9"/>
@@ -2366,15 +2420,15 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A55" s="5"/>
-      <c r="B55" s="12"/>
-      <c r="C55" s="11" t="s">
+      <c r="B55" s="11"/>
+      <c r="C55" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="D55" s="11" t="s">
+      <c r="D55" s="12" t="s">
         <v>207</v>
       </c>
-      <c r="E55" s="12" t="str">
-        <f t="shared" si="1"/>
+      <c r="E55" s="11" t="str">
+        <f t="shared" si="2"/>
         <v>GnrSrch.jsp</v>
       </c>
       <c r="F55" s="3" t="s">
@@ -2382,90 +2436,90 @@
       </c>
       <c r="G55" s="3"/>
       <c r="H55" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A56" s="5"/>
-      <c r="B56" s="12"/>
-      <c r="C56" s="11"/>
-      <c r="D56" s="11"/>
-      <c r="E56" s="12"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="12"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="11"/>
       <c r="F56" s="3" t="s">
         <v>183</v>
       </c>
       <c r="G56" s="3"/>
       <c r="H56" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A57" s="5"/>
-      <c r="B57" s="12"/>
-      <c r="C57" s="11"/>
-      <c r="D57" s="11"/>
-      <c r="E57" s="12"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="11"/>
       <c r="F57" s="3" t="s">
         <v>185</v>
       </c>
       <c r="G57" s="3"/>
       <c r="H57" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A58" s="5"/>
-      <c r="B58" s="12"/>
-      <c r="C58" s="11"/>
-      <c r="D58" s="11"/>
-      <c r="E58" s="12"/>
+      <c r="B58" s="11"/>
+      <c r="C58" s="12"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="11"/>
       <c r="F58" s="3" t="s">
         <v>186</v>
       </c>
       <c r="G58" s="3"/>
       <c r="H58" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A59" s="5"/>
-      <c r="B59" s="12"/>
-      <c r="C59" s="11"/>
-      <c r="D59" s="11"/>
-      <c r="E59" s="12"/>
+      <c r="B59" s="11"/>
+      <c r="C59" s="12"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="11"/>
       <c r="F59" s="8" t="s">
         <v>190</v>
       </c>
       <c r="G59" s="3"/>
       <c r="H59" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A60" s="5"/>
-      <c r="B60" s="12"/>
-      <c r="C60" s="11"/>
-      <c r="D60" s="11"/>
-      <c r="E60" s="12"/>
+      <c r="B60" s="11"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="11"/>
       <c r="F60" s="3" t="s">
         <v>184</v>
       </c>
       <c r="G60" s="3"/>
       <c r="H60" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A61" s="5"/>
-      <c r="B61" s="12"/>
-      <c r="C61" s="11" t="s">
+      <c r="B61" s="11"/>
+      <c r="C61" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="D61" s="11" t="s">
+      <c r="D61" s="12" t="s">
         <v>209</v>
       </c>
-      <c r="E61" s="12" t="str">
-        <f t="shared" si="1"/>
+      <c r="E61" s="11" t="str">
+        <f t="shared" si="2"/>
         <v>MonthSrch.jsp</v>
       </c>
       <c r="F61" s="3" t="s">
@@ -2476,10 +2530,10 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A62" s="5"/>
-      <c r="B62" s="12"/>
-      <c r="C62" s="11"/>
-      <c r="D62" s="11"/>
-      <c r="E62" s="12"/>
+      <c r="B62" s="11"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="12"/>
+      <c r="E62" s="11"/>
       <c r="F62" s="3" t="s">
         <v>183</v>
       </c>
@@ -2488,10 +2542,10 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A63" s="5"/>
-      <c r="B63" s="12"/>
-      <c r="C63" s="11"/>
-      <c r="D63" s="11"/>
-      <c r="E63" s="12"/>
+      <c r="B63" s="11"/>
+      <c r="C63" s="12"/>
+      <c r="D63" s="12"/>
+      <c r="E63" s="11"/>
       <c r="F63" s="3" t="s">
         <v>191</v>
       </c>
@@ -2502,15 +2556,15 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A64" s="5"/>
-      <c r="B64" s="12"/>
-      <c r="C64" s="11" t="s">
+      <c r="B64" s="11"/>
+      <c r="C64" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="D64" s="11" t="s">
+      <c r="D64" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="E64" s="12" t="str">
-        <f t="shared" si="1"/>
+      <c r="E64" s="11" t="str">
+        <f t="shared" si="2"/>
         <v>GnrResrv.jsp</v>
       </c>
       <c r="F64" s="3" t="s">
@@ -2521,10 +2575,10 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A65" s="5"/>
-      <c r="B65" s="12"/>
-      <c r="C65" s="11"/>
-      <c r="D65" s="11"/>
-      <c r="E65" s="12"/>
+      <c r="B65" s="11"/>
+      <c r="C65" s="12"/>
+      <c r="D65" s="12"/>
+      <c r="E65" s="11"/>
       <c r="F65" s="3" t="s">
         <v>210</v>
       </c>
@@ -2533,10 +2587,10 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A66" s="5"/>
-      <c r="B66" s="12"/>
-      <c r="C66" s="11"/>
-      <c r="D66" s="11"/>
-      <c r="E66" s="12"/>
+      <c r="B66" s="11"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="12"/>
+      <c r="E66" s="11"/>
       <c r="F66" s="3" t="s">
         <v>211</v>
       </c>
@@ -2545,10 +2599,10 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A67" s="5"/>
-      <c r="B67" s="12"/>
-      <c r="C67" s="11"/>
-      <c r="D67" s="11"/>
-      <c r="E67" s="12"/>
+      <c r="B67" s="11"/>
+      <c r="C67" s="12"/>
+      <c r="D67" s="12"/>
+      <c r="E67" s="11"/>
       <c r="F67" s="3" t="s">
         <v>212</v>
       </c>
@@ -2557,10 +2611,10 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A68" s="5"/>
-      <c r="B68" s="12"/>
-      <c r="C68" s="11"/>
-      <c r="D68" s="11"/>
-      <c r="E68" s="12"/>
+      <c r="B68" s="11"/>
+      <c r="C68" s="12"/>
+      <c r="D68" s="12"/>
+      <c r="E68" s="11"/>
       <c r="F68" s="8" t="s">
         <v>213</v>
       </c>
@@ -2569,10 +2623,10 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A69" s="5"/>
-      <c r="B69" s="12"/>
-      <c r="C69" s="11"/>
-      <c r="D69" s="11"/>
-      <c r="E69" s="12"/>
+      <c r="B69" s="11"/>
+      <c r="C69" s="12"/>
+      <c r="D69" s="12"/>
+      <c r="E69" s="11"/>
       <c r="F69" s="3" t="s">
         <v>185</v>
       </c>
@@ -2583,15 +2637,15 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A70" s="5"/>
-      <c r="B70" s="12"/>
-      <c r="C70" s="11" t="s">
+      <c r="B70" s="11"/>
+      <c r="C70" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="D70" s="11" t="s">
+      <c r="D70" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="E70" s="12" t="str">
-        <f t="shared" si="1"/>
+      <c r="E70" s="11" t="str">
+        <f t="shared" si="2"/>
         <v>PrgmSrch.jsp</v>
       </c>
       <c r="F70" s="3" t="s">
@@ -2602,10 +2656,10 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A71" s="5"/>
-      <c r="B71" s="12"/>
-      <c r="C71" s="11"/>
-      <c r="D71" s="11"/>
-      <c r="E71" s="12"/>
+      <c r="B71" s="11"/>
+      <c r="C71" s="12"/>
+      <c r="D71" s="12"/>
+      <c r="E71" s="11"/>
       <c r="F71" s="3" t="s">
         <v>183</v>
       </c>
@@ -2614,10 +2668,10 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A72" s="5"/>
-      <c r="B72" s="12"/>
-      <c r="C72" s="11"/>
-      <c r="D72" s="11"/>
-      <c r="E72" s="12"/>
+      <c r="B72" s="11"/>
+      <c r="C72" s="12"/>
+      <c r="D72" s="12"/>
+      <c r="E72" s="11"/>
       <c r="F72" s="3" t="s">
         <v>185</v>
       </c>
@@ -2626,10 +2680,10 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A73" s="5"/>
-      <c r="B73" s="12"/>
-      <c r="C73" s="11"/>
-      <c r="D73" s="11"/>
-      <c r="E73" s="12"/>
+      <c r="B73" s="11"/>
+      <c r="C73" s="12"/>
+      <c r="D73" s="12"/>
+      <c r="E73" s="11"/>
       <c r="F73" s="3" t="s">
         <v>186</v>
       </c>
@@ -2638,10 +2692,10 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A74" s="5"/>
-      <c r="B74" s="12"/>
-      <c r="C74" s="11"/>
-      <c r="D74" s="11"/>
-      <c r="E74" s="12"/>
+      <c r="B74" s="11"/>
+      <c r="C74" s="12"/>
+      <c r="D74" s="12"/>
+      <c r="E74" s="11"/>
       <c r="F74" s="8" t="s">
         <v>189</v>
       </c>
@@ -2650,15 +2704,15 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A75" s="5"/>
-      <c r="B75" s="12"/>
-      <c r="C75" s="11" t="s">
+      <c r="B75" s="11"/>
+      <c r="C75" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="D75" s="11" t="s">
+      <c r="D75" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="E75" s="12" t="str">
-        <f t="shared" si="1"/>
+      <c r="E75" s="11" t="str">
+        <f t="shared" si="2"/>
         <v>PrgmResrv.jsp</v>
       </c>
       <c r="F75" s="3" t="s">
@@ -2669,10 +2723,10 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A76" s="5"/>
-      <c r="B76" s="12"/>
-      <c r="C76" s="11"/>
-      <c r="D76" s="11"/>
-      <c r="E76" s="12"/>
+      <c r="B76" s="11"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
+      <c r="E76" s="11"/>
       <c r="F76" s="3" t="s">
         <v>214</v>
       </c>
@@ -2681,10 +2735,10 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A77" s="5"/>
-      <c r="B77" s="12"/>
-      <c r="C77" s="11"/>
-      <c r="D77" s="11"/>
-      <c r="E77" s="12"/>
+      <c r="B77" s="11"/>
+      <c r="C77" s="12"/>
+      <c r="D77" s="12"/>
+      <c r="E77" s="11"/>
       <c r="F77" s="3" t="s">
         <v>215</v>
       </c>
@@ -2693,10 +2747,10 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A78" s="5"/>
-      <c r="B78" s="12"/>
-      <c r="C78" s="11"/>
-      <c r="D78" s="11"/>
-      <c r="E78" s="12"/>
+      <c r="B78" s="11"/>
+      <c r="C78" s="12"/>
+      <c r="D78" s="12"/>
+      <c r="E78" s="11"/>
       <c r="F78" s="3" t="s">
         <v>217</v>
       </c>
@@ -2705,10 +2759,10 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A79" s="5"/>
-      <c r="B79" s="12"/>
-      <c r="C79" s="11"/>
-      <c r="D79" s="11"/>
-      <c r="E79" s="12"/>
+      <c r="B79" s="11"/>
+      <c r="C79" s="12"/>
+      <c r="D79" s="12"/>
+      <c r="E79" s="11"/>
       <c r="F79" s="3" t="s">
         <v>185</v>
       </c>
@@ -2719,15 +2773,15 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A80" s="5"/>
-      <c r="B80" s="12"/>
-      <c r="C80" s="11" t="s">
+      <c r="B80" s="11"/>
+      <c r="C80" s="12" t="s">
         <v>218</v>
       </c>
-      <c r="D80" s="11" t="s">
+      <c r="D80" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="E80" s="12" t="str">
-        <f t="shared" si="1"/>
+      <c r="E80" s="11" t="str">
+        <f t="shared" si="2"/>
         <v>PayInfo.jsp</v>
       </c>
       <c r="F80" s="3" t="s">
@@ -2738,10 +2792,10 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A81" s="5"/>
-      <c r="B81" s="12"/>
-      <c r="C81" s="11"/>
-      <c r="D81" s="11"/>
-      <c r="E81" s="12"/>
+      <c r="B81" s="11"/>
+      <c r="C81" s="12"/>
+      <c r="D81" s="12"/>
+      <c r="E81" s="11"/>
       <c r="F81" s="3" t="s">
         <v>222</v>
       </c>
@@ -2750,10 +2804,10 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A82" s="5"/>
-      <c r="B82" s="12"/>
-      <c r="C82" s="11"/>
-      <c r="D82" s="11"/>
-      <c r="E82" s="12"/>
+      <c r="B82" s="11"/>
+      <c r="C82" s="12"/>
+      <c r="D82" s="12"/>
+      <c r="E82" s="11"/>
       <c r="F82" s="3" t="s">
         <v>223</v>
       </c>
@@ -2762,10 +2816,10 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A83" s="5"/>
-      <c r="B83" s="12"/>
-      <c r="C83" s="11"/>
-      <c r="D83" s="11"/>
-      <c r="E83" s="12"/>
+      <c r="B83" s="11"/>
+      <c r="C83" s="12"/>
+      <c r="D83" s="12"/>
+      <c r="E83" s="11"/>
       <c r="F83" s="3" t="s">
         <v>224</v>
       </c>
@@ -2774,10 +2828,10 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A84" s="5"/>
-      <c r="B84" s="12"/>
-      <c r="C84" s="11"/>
-      <c r="D84" s="11"/>
-      <c r="E84" s="12"/>
+      <c r="B84" s="11"/>
+      <c r="C84" s="12"/>
+      <c r="D84" s="12"/>
+      <c r="E84" s="11"/>
       <c r="F84" s="3" t="s">
         <v>225</v>
       </c>
@@ -2786,7 +2840,7 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A85" s="5"/>
-      <c r="B85" s="12"/>
+      <c r="B85" s="11"/>
       <c r="C85" s="1" t="s">
         <v>227</v>
       </c>
@@ -2794,7 +2848,7 @@
         <v>228</v>
       </c>
       <c r="E85" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>PayCmplt.jsp</v>
       </c>
       <c r="F85" s="3" t="s">
@@ -2802,27 +2856,30 @@
       </c>
       <c r="G85" s="3"/>
       <c r="H85" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="48">
-    <mergeCell ref="B2:B85"/>
-    <mergeCell ref="C18:C22"/>
-    <mergeCell ref="D18:D22"/>
-    <mergeCell ref="E18:E22"/>
-    <mergeCell ref="E34:E36"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="E40:E42"/>
-    <mergeCell ref="E75:E79"/>
-    <mergeCell ref="E80:E84"/>
-    <mergeCell ref="E23:E26"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="E29:E32"/>
-    <mergeCell ref="D40:D42"/>
-    <mergeCell ref="C40:C42"/>
-    <mergeCell ref="E9:E14"/>
-    <mergeCell ref="E44:E48"/>
+  <mergeCells count="45">
+    <mergeCell ref="C80:C84"/>
+    <mergeCell ref="D80:D84"/>
+    <mergeCell ref="D75:D79"/>
+    <mergeCell ref="C75:C79"/>
+    <mergeCell ref="C70:C74"/>
+    <mergeCell ref="C2:C12"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="C61:C63"/>
+    <mergeCell ref="D61:D63"/>
+    <mergeCell ref="C44:C48"/>
+    <mergeCell ref="D44:D48"/>
+    <mergeCell ref="C49:C52"/>
+    <mergeCell ref="C55:C60"/>
+    <mergeCell ref="D55:D60"/>
+    <mergeCell ref="D14:D19"/>
+    <mergeCell ref="C14:C19"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
     <mergeCell ref="E55:E60"/>
     <mergeCell ref="E61:E63"/>
     <mergeCell ref="E64:E69"/>
@@ -2836,25 +2893,19 @@
     <mergeCell ref="D64:D69"/>
     <mergeCell ref="C64:C69"/>
     <mergeCell ref="D70:D74"/>
-    <mergeCell ref="C2:C7"/>
-    <mergeCell ref="D23:D26"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="C61:C63"/>
-    <mergeCell ref="D61:D63"/>
-    <mergeCell ref="C44:C48"/>
-    <mergeCell ref="D44:D48"/>
-    <mergeCell ref="C49:C52"/>
-    <mergeCell ref="C55:C60"/>
-    <mergeCell ref="D55:D60"/>
-    <mergeCell ref="D9:D14"/>
-    <mergeCell ref="C9:C14"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="C80:C84"/>
-    <mergeCell ref="D80:D84"/>
-    <mergeCell ref="D75:D79"/>
-    <mergeCell ref="C75:C79"/>
-    <mergeCell ref="C70:C74"/>
+    <mergeCell ref="B2:B85"/>
+    <mergeCell ref="E34:E36"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="E40:E42"/>
+    <mergeCell ref="E75:E79"/>
+    <mergeCell ref="E80:E84"/>
+    <mergeCell ref="E23:E26"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="E29:E32"/>
+    <mergeCell ref="D40:D42"/>
+    <mergeCell ref="C40:C42"/>
+    <mergeCell ref="E14:E19"/>
+    <mergeCell ref="E44:E48"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>